<commit_message>
join affiliations with CUG data via domain
</commit_message>
<xml_diff>
--- a/institutions.xlsx
+++ b/institutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D09B98-5DF8-8248-AC4A-EF2B3F3484E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F200D6D-8F3C-3E49-B85E-7DB878124196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
+    <workbookView xWindow="5580" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="148">
   <si>
     <t>domain</t>
   </si>
@@ -74,15 +74,9 @@
     <t>coventry</t>
   </si>
   <si>
-    <t>The Open University</t>
-  </si>
-  <si>
     <t>open</t>
   </si>
   <si>
-    <t>The University of Manchester</t>
-  </si>
-  <si>
     <t>manchester</t>
   </si>
   <si>
@@ -110,9 +104,6 @@
     <t>Falmouth University</t>
   </si>
   <si>
-    <t>The University of Edinburgh</t>
-  </si>
-  <si>
     <t>ed</t>
   </si>
   <si>
@@ -305,9 +296,6 @@
     <t>Heriot-Watt University</t>
   </si>
   <si>
-    <t>The University of Sheffield</t>
-  </si>
-  <si>
     <t>sheffield</t>
   </si>
   <si>
@@ -341,9 +329,6 @@
     <t>solent</t>
   </si>
   <si>
-    <t>Southampton Solent University</t>
-  </si>
-  <si>
     <t>southampton</t>
   </si>
   <si>
@@ -398,9 +383,6 @@
     <t>lboro</t>
   </si>
   <si>
-    <t>city</t>
-  </si>
-  <si>
     <t>City St George's, University of London</t>
   </si>
   <si>
@@ -464,15 +446,9 @@
     <t>Raspberry Pi Foundation</t>
   </si>
   <si>
-    <t>The Scottish Tech Army</t>
-  </si>
-  <si>
     <t>Theatr Na NOg</t>
   </si>
   <si>
-    <t>The Alan Turing Institute</t>
-  </si>
-  <si>
     <t>mdx</t>
   </si>
   <si>
@@ -480,6 +456,30 @@
   </si>
   <si>
     <t>Merton College</t>
+  </si>
+  <si>
+    <t>University of Manchester</t>
+  </si>
+  <si>
+    <t>University of Sheffield</t>
+  </si>
+  <si>
+    <t>Open University</t>
+  </si>
+  <si>
+    <t>Alan Turing Institute</t>
+  </si>
+  <si>
+    <t>Scottish Tech Army</t>
+  </si>
+  <si>
+    <t>University of Edinburgh</t>
+  </si>
+  <si>
+    <t>Northumbria University</t>
+  </si>
+  <si>
+    <t>Solent University</t>
   </si>
 </sst>
 </file>
@@ -872,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,654 +894,663 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>105</v>
+        <v>133</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>144</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>3</v>
+        <v>118</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>117</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>92</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>131</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="1"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="1"/>
+        <v>111</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>43</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>118</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>126</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="1"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C37" s="1"/>
+        <v>114</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C38" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>69</v>
+      <c r="A40" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>123</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>19</v>
+        <v>140</v>
       </c>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="3" t="s">
+      <c r="A44" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>135</v>
+      <c r="B46" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>83</v>
+        <v>9</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C48" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>74</v>
+        <v>146</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>82</v>
+      <c r="A51" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C51" s="1"/>
+        <v>63</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>89</v>
-      </c>
+      <c r="A52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="B53" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>103</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>133</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>112</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>5</v>
+        <v>78</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C60" s="1"/>
+        <v>131</v>
+      </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>96</v>
+        <v>130</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62" s="1"/>
+        <v>86</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C64" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C65" s="1"/>
+        <v>97</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C66" s="1"/>
+        <v>126</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>64</v>
+        <v>108</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>136</v>
+        <v>4</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>137</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>136</v>
+        <v>47</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>138</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>140</v>
+        <v>91</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>139</v>
+        <v>7</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>141</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>142</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B74" t="s">
-        <v>143</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B75" t="s">
-        <v>144</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>146</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B77" t="s">
-        <v>147</v>
+        <v>104</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C68">
-    <sortCondition ref="A2:A68"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C78">
+    <sortCondition ref="A2:A78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Weighted sums for comparison. HESA student numbers imported
</commit_message>
<xml_diff>
--- a/institutions.xlsx
+++ b/institutions.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F200D6D-8F3C-3E49-B85E-7DB878124196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C387549B-3371-7446-95B0-25E0A0F6A191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
+    <workbookView xWindow="2200" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$B$78</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -872,10 +875,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,633 +906,633 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>134</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>110</v>
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>69</v>
+        <v>116</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>99</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B13" t="s">
-        <v>143</v>
+        <v>99</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>133</v>
+        <v>11</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>133</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>135</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>133</v>
+      <c r="A16" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B17" t="s">
-        <v>136</v>
+        <v>20</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>128</v>
+        <v>52</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>119</v>
+        <v>39</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>14</v>
+        <v>94</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>145</v>
+        <v>50</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>114</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>3</v>
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>112</v>
+        <v>137</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>88</v>
+        <v>9</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>125</v>
+        <v>16</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>74</v>
+      <c r="A31" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>73</v>
+        <v>142</v>
       </c>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>105</v>
+        <v>133</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>113</v>
+        <v>133</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>120</v>
+        <v>38</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>50</v>
+        <v>133</v>
+      </c>
+      <c r="B42" t="s">
+        <v>136</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>140</v>
+        <v>59</v>
       </c>
       <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>138</v>
+        <v>25</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>27</v>
+        <v>109</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>66</v>
+      <c r="A46" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>17</v>
+        <v>118</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>64</v>
+      <c r="A51" s="2" t="s">
+        <v>2</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>142</v>
+      <c r="A52" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" t="s">
-        <v>139</v>
+        <v>124</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>129</v>
+        <v>74</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="C55" s="1"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>57</v>
+        <v>106</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>18</v>
+        <v>121</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>130</v>
+        <v>13</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>141</v>
+      <c r="A62" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>37</v>
+        <v>93</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="C63" s="1"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>147</v>
+        <v>80</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>126</v>
+        <v>86</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>24</v>
+        <v>126</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C67" s="1"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>48</v>
+        <v>108</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="C70" s="1"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>92</v>
+        <v>4</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>44</v>
+        <v>91</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>59</v>
+        <v>89</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>76</v>
+        <v>36</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="C76" s="1"/>
     </row>
@@ -1549,8 +1553,80 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C78">
-    <sortCondition ref="A2:A78"/>
+  <autoFilter ref="A2:B78" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="aber"/>
+        <filter val="abertay"/>
+        <filter val="arts"/>
+        <filter val="aston"/>
+        <filter val="bath"/>
+        <filter val="bcu"/>
+        <filter val="bristol"/>
+        <filter val="brookes"/>
+        <filter val="cam"/>
+        <filter val="cardiff"/>
+        <filter val="chester"/>
+        <filter val="citystgeorges"/>
+        <filter val="coventry"/>
+        <filter val="dundee"/>
+        <filter val="durham"/>
+        <filter val="ed"/>
+        <filter val="falmouth"/>
+        <filter val="gcu"/>
+        <filter val="gla"/>
+        <filter val="glos"/>
+        <filter val="gold"/>
+        <filter val="herts"/>
+        <filter val="hud"/>
+        <filter val="hull"/>
+        <filter val="hw"/>
+        <filter val="kcl"/>
+        <filter val="kent"/>
+        <filter val="lancaster"/>
+        <filter val="lboro"/>
+        <filter val="leeds"/>
+        <filter val="leedstrinity"/>
+        <filter val="lincoln"/>
+        <filter val="liverpool"/>
+        <filter val="lse"/>
+        <filter val="manchester"/>
+        <filter val="mdx"/>
+        <filter val="mmu"/>
+        <filter val="napier"/>
+        <filter val="ncl"/>
+        <filter val="newman"/>
+        <filter val="northumbria"/>
+        <filter val="nottingham"/>
+        <filter val="open"/>
+        <filter val="ox"/>
+        <filter val="port"/>
+        <filter val="qmul"/>
+        <filter val="qub"/>
+        <filter val="rgu"/>
+        <filter val="roehampton"/>
+        <filter val="sheffield"/>
+        <filter val="shu"/>
+        <filter val="solent"/>
+        <filter val="southampton"/>
+        <filter val="southwales"/>
+        <filter val="st-andrews"/>
+        <filter val="stir"/>
+        <filter val="strath"/>
+        <filter val="sunderland"/>
+        <filter val="sussex"/>
+        <filter val="swansea"/>
+        <filter val="uclan"/>
+        <filter val="ulster"/>
+        <filter val="uwl"/>
+        <filter val="warwick"/>
+        <filter val="york"/>
+        <filter val="yorksj"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B78">
+    <sortCondition ref="B3:B78"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Linked missing student number data
</commit_message>
<xml_diff>
--- a/institutions.xlsx
+++ b/institutions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C387549B-3371-7446-95B0-25E0A0F6A191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEF62CE-64A7-014F-8937-8D19B4DB5707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$B$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$B$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="151">
   <si>
     <t>domain</t>
   </si>
@@ -483,6 +483,15 @@
   </si>
   <si>
     <t>Solent University</t>
+  </si>
+  <si>
+    <t>University of Durham</t>
+  </si>
+  <si>
+    <t>University of Lancaster</t>
+  </si>
+  <si>
+    <t>University of St. Andrews</t>
   </si>
 </sst>
 </file>
@@ -876,10 +885,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B78"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,543 +1026,568 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>51</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>88</v>
+        <v>52</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>85</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>149</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B27" t="s">
-        <v>139</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>8</v>
+        <v>93</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>146</v>
+        <v>137</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>12</v>
+      <c r="A31" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="C31" s="1"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="1"/>
+        <v>146</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>58</v>
+      <c r="A33" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>133</v>
+        <v>58</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>135</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B42" t="s">
-        <v>136</v>
+        <v>130</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>26</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B44" t="s">
+        <v>136</v>
+      </c>
+      <c r="C44" s="1"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>110</v>
+        <v>60</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="C45" s="1"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>44</v>
+        <v>109</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>128</v>
+        <v>54</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>119</v>
+        <v>43</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="C50" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>3</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>112</v>
+        <v>22</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>125</v>
+        <v>2</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>73</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="1"/>
+        <v>124</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C56" s="1"/>
+        <v>74</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>120</v>
+        <v>42</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="C57" s="1"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>83</v>
+        <v>106</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>67</v>
+        <v>121</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>140</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
-        <v>64</v>
+      <c r="A62" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="C63" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>80</v>
+      <c r="A64" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>78</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C65" s="1"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>141</v>
+        <v>80</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="C67" s="1"/>
+        <v>79</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>98</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>24</v>
+        <v>126</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C70" s="1"/>
+        <v>98</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C73" s="1"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C74" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="C75" s="1"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>35</v>
+        <v>91</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>103</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:B78" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
+  <autoFilter ref="A2:B81" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
     <filterColumn colId="0">
       <filters>
         <filter val="aber"/>
@@ -1625,8 +1659,8 @@
       </filters>
     </filterColumn>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B78">
-    <sortCondition ref="B3:B78"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B81">
+    <sortCondition ref="B3:B81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
CUG data weighted by student numbers, ECDF graphs done
</commit_message>
<xml_diff>
--- a/institutions.xlsx
+++ b/institutions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcs0spb/Software/CEP_Retro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEF62CE-64A7-014F-8937-8D19B4DB5707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C630E0E-039A-434C-91A7-73DE113010F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
+    <workbookView xWindow="8560" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{6EE73B8C-4C57-1F4E-A40F-8D5585F0E2F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="260">
   <si>
     <t>domain</t>
   </si>
@@ -305,15 +305,9 @@
     <t>gold</t>
   </si>
   <si>
-    <t>Goldsmiths, University of London</t>
-  </si>
-  <si>
     <t>arts</t>
   </si>
   <si>
-    <t>University of the Arts London</t>
-  </si>
-  <si>
     <t>sussex</t>
   </si>
   <si>
@@ -492,6 +486,339 @@
   </si>
   <si>
     <t>University of St. Andrews</t>
+  </si>
+  <si>
+    <t>Goldsmiths</t>
+  </si>
+  <si>
+    <t>University of the Arts</t>
+  </si>
+  <si>
+    <t>Teesside University</t>
+  </si>
+  <si>
+    <t>tees</t>
+  </si>
+  <si>
+    <t>De Montfort University</t>
+  </si>
+  <si>
+    <t>dmu</t>
+  </si>
+  <si>
+    <t>University of the West of England</t>
+  </si>
+  <si>
+    <t>uwe</t>
+  </si>
+  <si>
+    <t>University of Greenwich</t>
+  </si>
+  <si>
+    <t>gre</t>
+  </si>
+  <si>
+    <t>Staffordshire University</t>
+  </si>
+  <si>
+    <t>staffs</t>
+  </si>
+  <si>
+    <t>University of Westminster</t>
+  </si>
+  <si>
+    <t>westminster</t>
+  </si>
+  <si>
+    <t>Bournemouth University</t>
+  </si>
+  <si>
+    <t>bournemouth</t>
+  </si>
+  <si>
+    <t>University of Birmingham</t>
+  </si>
+  <si>
+    <t>birmingham</t>
+  </si>
+  <si>
+    <t>Kingston University</t>
+  </si>
+  <si>
+    <t>kingston</t>
+  </si>
+  <si>
+    <t>University of East London</t>
+  </si>
+  <si>
+    <t>uel</t>
+  </si>
+  <si>
+    <t>Nottingham Trent University</t>
+  </si>
+  <si>
+    <t>ntu</t>
+  </si>
+  <si>
+    <t>Brunel University</t>
+  </si>
+  <si>
+    <t>brunel</t>
+  </si>
+  <si>
+    <t>University of Leicester</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>Anglia Ruskin University</t>
+  </si>
+  <si>
+    <t>aru</t>
+  </si>
+  <si>
+    <t>Royal Holloway</t>
+  </si>
+  <si>
+    <t>royalholloway</t>
+  </si>
+  <si>
+    <t>University of the West of Scotland</t>
+  </si>
+  <si>
+    <t>uws</t>
+  </si>
+  <si>
+    <t>Arden University</t>
+  </si>
+  <si>
+    <t>arden</t>
+  </si>
+  <si>
+    <t>Leeds Beckett University</t>
+  </si>
+  <si>
+    <t>leedsbeckett</t>
+  </si>
+  <si>
+    <t>exeter</t>
+  </si>
+  <si>
+    <t>University of Exeter</t>
+  </si>
+  <si>
+    <t>University of Salford</t>
+  </si>
+  <si>
+    <t>salford</t>
+  </si>
+  <si>
+    <t>University of Wolverhampton</t>
+  </si>
+  <si>
+    <t>wlv</t>
+  </si>
+  <si>
+    <t>University of Bedfordshire</t>
+  </si>
+  <si>
+    <t>beds</t>
+  </si>
+  <si>
+    <t>cardiffmet</t>
+  </si>
+  <si>
+    <t>Cardiff Metropolitan University</t>
+  </si>
+  <si>
+    <t>University of Derby</t>
+  </si>
+  <si>
+    <t>derby</t>
+  </si>
+  <si>
+    <t>Roehampton University</t>
+  </si>
+  <si>
+    <t>University of Bradford</t>
+  </si>
+  <si>
+    <t>bradford</t>
+  </si>
+  <si>
+    <t>University of Essex</t>
+  </si>
+  <si>
+    <t>essex</t>
+  </si>
+  <si>
+    <t>greatermanchester</t>
+  </si>
+  <si>
+    <t>University of Bolton</t>
+  </si>
+  <si>
+    <t>Liverpool John Moores University</t>
+  </si>
+  <si>
+    <t>ljmu</t>
+  </si>
+  <si>
+    <t>University of East Anglia</t>
+  </si>
+  <si>
+    <t>uea</t>
+  </si>
+  <si>
+    <t>uca</t>
+  </si>
+  <si>
+    <t>University for the Creative Arts</t>
+  </si>
+  <si>
+    <t>University of Wales Trinity Saint David</t>
+  </si>
+  <si>
+    <t>uwtsd</t>
+  </si>
+  <si>
+    <t>northampton</t>
+  </si>
+  <si>
+    <t>University of Northampton</t>
+  </si>
+  <si>
+    <t>lsbu</t>
+  </si>
+  <si>
+    <t>London South Bank University</t>
+  </si>
+  <si>
+    <t>Keele University</t>
+  </si>
+  <si>
+    <t>keele</t>
+  </si>
+  <si>
+    <t>University of Brighton</t>
+  </si>
+  <si>
+    <t>brighton</t>
+  </si>
+  <si>
+    <t>University of Surrey</t>
+  </si>
+  <si>
+    <t>surrey</t>
+  </si>
+  <si>
+    <t>Edge Hill University</t>
+  </si>
+  <si>
+    <t>edgehill</t>
+  </si>
+  <si>
+    <t>bbk</t>
+  </si>
+  <si>
+    <t>Birkbeck College</t>
+  </si>
+  <si>
+    <t>University of Plymouth</t>
+  </si>
+  <si>
+    <t>plymouth</t>
+  </si>
+  <si>
+    <t>uos</t>
+  </si>
+  <si>
+    <t>University of Suffolk</t>
+  </si>
+  <si>
+    <t>londonmet</t>
+  </si>
+  <si>
+    <t>London Metropolitan University</t>
+  </si>
+  <si>
+    <t>wrexham</t>
+  </si>
+  <si>
+    <t>Wrexham University</t>
+  </si>
+  <si>
+    <t>bucks</t>
+  </si>
+  <si>
+    <t>Buckinghamshire New University</t>
+  </si>
+  <si>
+    <t>buckingham</t>
+  </si>
+  <si>
+    <t>University of Buckingham</t>
+  </si>
+  <si>
+    <t>canterbury</t>
+  </si>
+  <si>
+    <t>Canterbury Christ Church University</t>
+  </si>
+  <si>
+    <t>worcester</t>
+  </si>
+  <si>
+    <t>University of Worcester</t>
+  </si>
+  <si>
+    <t>chi</t>
+  </si>
+  <si>
+    <t>University of Chichester</t>
+  </si>
+  <si>
+    <t>hope</t>
+  </si>
+  <si>
+    <t>Liverpool Hope University</t>
+  </si>
+  <si>
+    <t>bathspa</t>
+  </si>
+  <si>
+    <t>Bath Spa University</t>
+  </si>
+  <si>
+    <t>bangor</t>
+  </si>
+  <si>
+    <t>Bangor University</t>
+  </si>
+  <si>
+    <t>winchester</t>
+  </si>
+  <si>
+    <t>University of Winchester</t>
+  </si>
+  <si>
+    <t>reading</t>
+  </si>
+  <si>
+    <t>University of Reading</t>
+  </si>
+  <si>
+    <t>ucl</t>
+  </si>
+  <si>
+    <t>University College London</t>
+  </si>
+  <si>
+    <t>imperial</t>
+  </si>
+  <si>
+    <t>Imperial College London</t>
   </si>
 </sst>
 </file>
@@ -884,16 +1211,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A137" sqref="A137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -907,10 +1233,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,36 +1250,36 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -976,10 +1302,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -994,19 +1320,19 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1030,7 +1356,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1062,7 +1388,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1095,15 +1421,15 @@
         <v>39</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -1118,10 +1444,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C27" s="1"/>
     </row>
@@ -1136,18 +1462,18 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1163,7 +1489,7 @@
         <v>16</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1171,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C33" s="1"/>
     </row>
@@ -1202,12 +1528,12 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1218,12 +1544,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1236,18 +1562,18 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="3" t="s">
         <v>130</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>132</v>
       </c>
       <c r="C42" s="1"/>
     </row>
@@ -1260,12 +1586,12 @@
       </c>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C44" s="1"/>
     </row>
@@ -1288,10 +1614,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C47" s="1"/>
     </row>
@@ -1314,18 +1640,18 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C51" s="1"/>
     </row>
@@ -1334,7 +1660,7 @@
         <v>22</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C52" s="1"/>
     </row>
@@ -1348,19 +1674,19 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C54" s="1"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
@@ -1382,19 +1708,19 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C58" s="1"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" s="1"/>
     </row>
@@ -1421,7 +1747,7 @@
         <v>13</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -1442,10 +1768,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C65" s="1"/>
     </row>
@@ -1470,24 +1796,24 @@
         <v>86</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C69" s="1"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
@@ -1504,16 +1830,16 @@
         <v>23</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C72" s="1"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C73" s="1"/>
     </row>
@@ -1536,19 +1862,19 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C76" s="1"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="C77" s="1"/>
     </row>
@@ -1572,10 +1898,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1586,79 +1912,449 @@
         <v>61</v>
       </c>
     </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A92" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A93" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A94" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A95" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C117" s="1"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A134" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A135" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:B81" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="aber"/>
-        <filter val="abertay"/>
-        <filter val="arts"/>
-        <filter val="aston"/>
-        <filter val="bath"/>
-        <filter val="bcu"/>
-        <filter val="bristol"/>
-        <filter val="brookes"/>
-        <filter val="cam"/>
-        <filter val="cardiff"/>
-        <filter val="chester"/>
-        <filter val="citystgeorges"/>
-        <filter val="coventry"/>
-        <filter val="dundee"/>
-        <filter val="durham"/>
-        <filter val="ed"/>
-        <filter val="falmouth"/>
-        <filter val="gcu"/>
-        <filter val="gla"/>
-        <filter val="glos"/>
-        <filter val="gold"/>
-        <filter val="herts"/>
-        <filter val="hud"/>
-        <filter val="hull"/>
-        <filter val="hw"/>
-        <filter val="kcl"/>
-        <filter val="kent"/>
-        <filter val="lancaster"/>
-        <filter val="lboro"/>
-        <filter val="leeds"/>
-        <filter val="leedstrinity"/>
-        <filter val="lincoln"/>
-        <filter val="liverpool"/>
-        <filter val="lse"/>
-        <filter val="manchester"/>
-        <filter val="mdx"/>
-        <filter val="mmu"/>
-        <filter val="napier"/>
-        <filter val="ncl"/>
-        <filter val="newman"/>
-        <filter val="northumbria"/>
-        <filter val="nottingham"/>
-        <filter val="open"/>
-        <filter val="ox"/>
-        <filter val="port"/>
-        <filter val="qmul"/>
-        <filter val="qub"/>
-        <filter val="rgu"/>
-        <filter val="roehampton"/>
-        <filter val="sheffield"/>
-        <filter val="shu"/>
-        <filter val="solent"/>
-        <filter val="southampton"/>
-        <filter val="southwales"/>
-        <filter val="st-andrews"/>
-        <filter val="stir"/>
-        <filter val="strath"/>
-        <filter val="sunderland"/>
-        <filter val="sussex"/>
-        <filter val="swansea"/>
-        <filter val="uclan"/>
-        <filter val="ulster"/>
-        <filter val="uwl"/>
-        <filter val="warwick"/>
-        <filter val="york"/>
-        <filter val="yorksj"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:B81" xr:uid="{38947F36-5E62-2E4B-8218-4957026C99B0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B81">
     <sortCondition ref="B3:B81"/>
   </sortState>

</xml_diff>